<commit_message>
Add LOG2(M+1) column for comparison
</commit_message>
<xml_diff>
--- a/hw2/problem2.xlsx
+++ b/hw2/problem2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="6">
   <si>
     <t>N</t>
   </si>
@@ -30,10 +30,13 @@
     <t>LEN(result)</t>
   </si>
   <si>
-    <t>N+Log2(m)</t>
+    <t>LEN(binary)</t>
   </si>
   <si>
-    <t>LEN(binary)</t>
+    <t>N+Log2(M+1)</t>
+  </si>
+  <si>
+    <t>N+Log2(M)</t>
   </si>
 </sst>
 </file>
@@ -371,15 +374,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC12"/>
+  <dimension ref="A1:AH12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,78 +390,93 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
       </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
       <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
         <v>0</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>1</v>
       </c>
-      <c r="P1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>3</v>
       </c>
       <c r="S1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" t="s">
         <v>0</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>1</v>
       </c>
-      <c r="V1" t="s">
-        <v>4</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC1" t="s">
         <v>0</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AD1" t="s">
         <v>1</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AF1" t="s">
         <v>2</v>
       </c>
-      <c r="AC1" t="s">
-        <v>3</v>
+      <c r="AG1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>3</v>
       </c>
-      <c r="M2" s="1">
-        <v>4</v>
-      </c>
-      <c r="S2" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y2" s="1">
+      <c r="O2" s="1">
+        <v>4</v>
+      </c>
+      <c r="V2" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC2" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>B3*(2^A$2-1)</f>
         <v>3</v>
@@ -478,84 +496,104 @@
         <f>A$2+_xlfn.CEILING.MATH(LOG(B3,2))</f>
         <v>2</v>
       </c>
-      <c r="G3">
-        <f>H3*(2^G$2-1)</f>
-        <v>7</v>
+      <c r="F3">
+        <f>A$2+_xlfn.CEILING.MATH(LOG(B3+1,2))</f>
+        <v>3</v>
       </c>
       <c r="H3">
+        <f>I3*(2^H$2-1)</f>
+        <v>7</v>
+      </c>
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="I3" t="str">
-        <f>DEC2BIN(G3)</f>
+      <c r="J3" t="str">
+        <f>DEC2BIN(H3)</f>
         <v>111</v>
       </c>
-      <c r="J3">
-        <f>LEN(I3)</f>
+      <c r="K3">
+        <f>LEN(J3)</f>
         <v>3</v>
       </c>
-      <c r="K3">
-        <f>G$2+_xlfn.CEILING.MATH(LOG(H3,2))</f>
+      <c r="L3">
+        <f>H$2+_xlfn.CEILING.MATH(LOG(I3,2))</f>
         <v>3</v>
       </c>
       <c r="M3">
-        <f>N3*(2^M$2-1)</f>
+        <f>H$2+_xlfn.CEILING.MATH(LOG(I3+1,2))</f>
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <f>P3*(2^O$2-1)</f>
         <v>15</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>1</v>
       </c>
-      <c r="O3" t="str">
-        <f>DEC2BIN(M3)</f>
+      <c r="Q3" t="str">
+        <f>DEC2BIN(O3)</f>
         <v>1111</v>
       </c>
-      <c r="P3">
-        <f>LEN(O3)</f>
-        <v>4</v>
-      </c>
-      <c r="Q3">
-        <f>M$2+_xlfn.CEILING.MATH(LOG(N3,2))</f>
+      <c r="R3">
+        <f>LEN(Q3)</f>
         <v>4</v>
       </c>
       <c r="S3">
-        <f>T3*(2^S$2-1)</f>
+        <f>O$2+_xlfn.CEILING.MATH(LOG(P3,2))</f>
+        <v>4</v>
+      </c>
+      <c r="T3">
+        <f>O$2+_xlfn.CEILING.MATH(LOG(P3+1,2))</f>
+        <v>5</v>
+      </c>
+      <c r="V3">
+        <f>W3*(2^V$2-1)</f>
         <v>31</v>
       </c>
-      <c r="T3">
+      <c r="W3">
         <v>1</v>
       </c>
-      <c r="U3" t="str">
-        <f>DEC2BIN(S3)</f>
+      <c r="X3" t="str">
+        <f>DEC2BIN(V3)</f>
         <v>11111</v>
       </c>
-      <c r="V3">
-        <f>LEN(U3)</f>
-        <v>5</v>
-      </c>
-      <c r="W3">
-        <f>S$2+_xlfn.CEILING.MATH(LOG(T3,2))</f>
-        <v>5</v>
-      </c>
       <c r="Y3">
-        <f>Z3*(2^Y$2-1)</f>
+        <f>LEN(X3)</f>
+        <v>5</v>
+      </c>
+      <c r="Z3">
+        <f>V$2+_xlfn.CEILING.MATH(LOG(W3,2))</f>
+        <v>5</v>
+      </c>
+      <c r="AA3">
+        <f>V$2+_xlfn.CEILING.MATH(LOG(W3+1,2))</f>
+        <v>6</v>
+      </c>
+      <c r="AC3">
+        <f>AD3*(2^AC$2-1)</f>
         <v>63</v>
       </c>
-      <c r="Z3">
+      <c r="AD3">
         <v>1</v>
       </c>
-      <c r="AA3" t="str">
-        <f>DEC2BIN(Y3)</f>
+      <c r="AE3" t="str">
+        <f>DEC2BIN(AC3)</f>
         <v>111111</v>
       </c>
-      <c r="AB3">
-        <f>LEN(AA3)</f>
-        <v>6</v>
-      </c>
-      <c r="AC3">
-        <f>Y$2+_xlfn.CEILING.MATH(LOG(Z3,2))</f>
-        <v>6</v>
+      <c r="AF3">
+        <f>LEN(AE3)</f>
+        <v>6</v>
+      </c>
+      <c r="AG3">
+        <f>AC$2+_xlfn.CEILING.MATH(LOG(AD3,2))</f>
+        <v>6</v>
+      </c>
+      <c r="AH3">
+        <f>AC$2+_xlfn.CEILING.MATH(LOG(AD3+1,2))</f>
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">B4*(2^A$2-1)</f>
         <v>6</v>
@@ -575,84 +613,104 @@
         <f t="shared" ref="E4:E12" si="3">A$2+_xlfn.CEILING.MATH(LOG(B4,2))</f>
         <v>3</v>
       </c>
-      <c r="G4">
-        <f t="shared" ref="G4:G12" si="4">H4*(2^G$2-1)</f>
+      <c r="F4">
+        <f t="shared" ref="F4:F12" si="4">A$2+_xlfn.CEILING.MATH(LOG(B4+1,2))</f>
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H12" si="5">I4*(2^H$2-1)</f>
         <v>14</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="I4" t="str">
-        <f t="shared" ref="I4:I12" si="5">DEC2BIN(G4)</f>
+      <c r="J4" t="str">
+        <f t="shared" ref="J4:J12" si="6">DEC2BIN(H4)</f>
         <v>1110</v>
       </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J12" si="6">LEN(I4)</f>
-        <v>4</v>
-      </c>
       <c r="K4">
-        <f t="shared" ref="K4:K12" si="7">G$2+_xlfn.CEILING.MATH(LOG(H4,2))</f>
+        <f t="shared" ref="K4:K12" si="7">LEN(J4)</f>
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L12" si="8">H$2+_xlfn.CEILING.MATH(LOG(I4,2))</f>
         <v>4</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M12" si="8">N4*(2^M$2-1)</f>
+        <f t="shared" ref="M4:M12" si="9">H$2+_xlfn.CEILING.MATH(LOG(I4+1,2))</f>
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O12" si="10">P4*(2^O$2-1)</f>
         <v>30</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>2</v>
       </c>
-      <c r="O4" t="str">
-        <f t="shared" ref="O4:O12" si="9">DEC2BIN(M4)</f>
+      <c r="Q4" t="str">
+        <f t="shared" ref="Q4:Q12" si="11">DEC2BIN(O4)</f>
         <v>11110</v>
       </c>
-      <c r="P4">
-        <f t="shared" ref="P4:P12" si="10">LEN(O4)</f>
-        <v>5</v>
-      </c>
-      <c r="Q4">
-        <f t="shared" ref="Q4:Q12" si="11">M$2+_xlfn.CEILING.MATH(LOG(N4,2))</f>
+      <c r="R4">
+        <f t="shared" ref="R4:R12" si="12">LEN(Q4)</f>
         <v>5</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:S12" si="12">T4*(2^S$2-1)</f>
+        <f t="shared" ref="S4:S12" si="13">O$2+_xlfn.CEILING.MATH(LOG(P4,2))</f>
+        <v>5</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T12" si="14">O$2+_xlfn.CEILING.MATH(LOG(P4+1,2))</f>
+        <v>6</v>
+      </c>
+      <c r="V4">
+        <f t="shared" ref="V4:V12" si="15">W4*(2^V$2-1)</f>
         <v>62</v>
       </c>
-      <c r="T4">
+      <c r="W4">
         <v>2</v>
       </c>
-      <c r="U4" t="str">
-        <f t="shared" ref="U4:U12" si="13">DEC2BIN(S4)</f>
+      <c r="X4" t="str">
+        <f t="shared" ref="X4:X12" si="16">DEC2BIN(V4)</f>
         <v>111110</v>
       </c>
-      <c r="V4">
-        <f t="shared" ref="V4:V12" si="14">LEN(U4)</f>
-        <v>6</v>
-      </c>
-      <c r="W4">
-        <f t="shared" ref="W4:W12" si="15">S$2+_xlfn.CEILING.MATH(LOG(T4,2))</f>
-        <v>6</v>
-      </c>
       <c r="Y4">
-        <f t="shared" ref="Y4:Y12" si="16">Z4*(2^Y$2-1)</f>
+        <f t="shared" ref="Y4:Y12" si="17">LEN(X4)</f>
+        <v>6</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" ref="Z4:Z12" si="18">V$2+_xlfn.CEILING.MATH(LOG(W4,2))</f>
+        <v>6</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" ref="AA4:AA12" si="19">V$2+_xlfn.CEILING.MATH(LOG(W4+1,2))</f>
+        <v>7</v>
+      </c>
+      <c r="AC4">
+        <f t="shared" ref="AC4:AC12" si="20">AD4*(2^AC$2-1)</f>
         <v>126</v>
       </c>
-      <c r="Z4">
+      <c r="AD4">
         <v>2</v>
       </c>
-      <c r="AA4" t="str">
-        <f t="shared" ref="AA4:AA12" si="17">DEC2BIN(Y4)</f>
+      <c r="AE4" t="str">
+        <f t="shared" ref="AE4:AE12" si="21">DEC2BIN(AC4)</f>
         <v>1111110</v>
       </c>
-      <c r="AB4">
-        <f t="shared" ref="AB4:AB12" si="18">LEN(AA4)</f>
-        <v>7</v>
-      </c>
-      <c r="AC4">
-        <f t="shared" ref="AC4:AC12" si="19">Y$2+_xlfn.CEILING.MATH(LOG(Z4,2))</f>
-        <v>7</v>
+      <c r="AF4">
+        <f t="shared" ref="AF4:AF12" si="22">LEN(AE4)</f>
+        <v>7</v>
+      </c>
+      <c r="AG4">
+        <f t="shared" ref="AG4:AG12" si="23">AC$2+_xlfn.CEILING.MATH(LOG(AD4,2))</f>
+        <v>7</v>
+      </c>
+      <c r="AH4">
+        <f t="shared" ref="AH4:AH12" si="24">AC$2+_xlfn.CEILING.MATH(LOG(AD4+1,2))</f>
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -672,84 +730,104 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="G5">
+      <c r="F5">
         <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>3</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="5"/>
+      <c r="J5" t="str">
+        <f t="shared" si="6"/>
         <v>10101</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="6"/>
-        <v>5</v>
       </c>
       <c r="K5">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
+      <c r="L5">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
       <c r="M5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="10"/>
         <v>45</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>3</v>
       </c>
-      <c r="O5" t="str">
-        <f t="shared" si="9"/>
+      <c r="Q5" t="str">
+        <f t="shared" si="11"/>
         <v>101101</v>
       </c>
-      <c r="P5">
-        <f t="shared" si="10"/>
-        <v>6</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="11"/>
+      <c r="R5">
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="S5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="15"/>
         <v>93</v>
       </c>
-      <c r="T5">
+      <c r="W5">
         <v>3</v>
       </c>
-      <c r="U5" t="str">
-        <f t="shared" si="13"/>
+      <c r="X5" t="str">
+        <f t="shared" si="16"/>
         <v>1011101</v>
       </c>
-      <c r="V5">
-        <f t="shared" si="14"/>
-        <v>7</v>
-      </c>
-      <c r="W5">
-        <f t="shared" si="15"/>
-        <v>7</v>
-      </c>
       <c r="Y5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="18"/>
+        <v>7</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="19"/>
+        <v>7</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" si="20"/>
         <v>189</v>
       </c>
-      <c r="Z5">
+      <c r="AD5">
         <v>3</v>
       </c>
-      <c r="AA5" t="str">
-        <f t="shared" si="17"/>
+      <c r="AE5" t="str">
+        <f t="shared" si="21"/>
         <v>10111101</v>
       </c>
-      <c r="AB5">
-        <f t="shared" si="18"/>
-        <v>8</v>
-      </c>
-      <c r="AC5">
-        <f t="shared" si="19"/>
+      <c r="AF5">
+        <f t="shared" si="22"/>
+        <v>8</v>
+      </c>
+      <c r="AG5">
+        <f t="shared" si="23"/>
+        <v>8</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -769,84 +847,104 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="G6">
+      <c r="F6">
         <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="H6">
-        <v>4</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="5"/>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="6"/>
         <v>11100</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="6"/>
-        <v>5</v>
       </c>
       <c r="K6">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
+      <c r="L6">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
       <c r="M6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="10"/>
         <v>60</v>
       </c>
-      <c r="N6">
-        <v>4</v>
-      </c>
-      <c r="O6" t="str">
-        <f t="shared" si="9"/>
+      <c r="P6">
+        <v>4</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="11"/>
         <v>111100</v>
       </c>
-      <c r="P6">
-        <f t="shared" si="10"/>
-        <v>6</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="11"/>
+      <c r="R6">
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="S6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="14"/>
+        <v>7</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="15"/>
         <v>124</v>
       </c>
-      <c r="T6">
-        <v>4</v>
-      </c>
-      <c r="U6" t="str">
-        <f t="shared" si="13"/>
+      <c r="W6">
+        <v>4</v>
+      </c>
+      <c r="X6" t="str">
+        <f t="shared" si="16"/>
         <v>1111100</v>
       </c>
-      <c r="V6">
-        <f t="shared" si="14"/>
-        <v>7</v>
-      </c>
-      <c r="W6">
-        <f t="shared" si="15"/>
-        <v>7</v>
-      </c>
       <c r="Y6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="18"/>
+        <v>7</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="19"/>
+        <v>8</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="20"/>
         <v>252</v>
       </c>
-      <c r="Z6">
-        <v>4</v>
-      </c>
-      <c r="AA6" t="str">
-        <f t="shared" si="17"/>
+      <c r="AD6">
+        <v>4</v>
+      </c>
+      <c r="AE6" t="str">
+        <f t="shared" si="21"/>
         <v>11111100</v>
       </c>
-      <c r="AB6">
-        <f t="shared" si="18"/>
-        <v>8</v>
-      </c>
-      <c r="AC6">
-        <f t="shared" si="19"/>
-        <v>8</v>
+      <c r="AF6">
+        <f t="shared" si="22"/>
+        <v>8</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" si="23"/>
+        <v>8</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" si="24"/>
+        <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -866,84 +964,104 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="G7">
+      <c r="F7">
         <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="5"/>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="6"/>
         <v>100011</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="6"/>
-        <v>6</v>
       </c>
       <c r="K7">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
+      <c r="L7">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
       <c r="M7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="N7">
-        <v>5</v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" si="9"/>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="11"/>
         <v>1001011</v>
       </c>
-      <c r="P7">
-        <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="11"/>
+      <c r="R7">
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="S7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="14"/>
+        <v>7</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="15"/>
         <v>155</v>
       </c>
-      <c r="T7">
-        <v>5</v>
-      </c>
-      <c r="U7" t="str">
-        <f t="shared" si="13"/>
+      <c r="W7">
+        <v>5</v>
+      </c>
+      <c r="X7" t="str">
+        <f t="shared" si="16"/>
         <v>10011011</v>
       </c>
-      <c r="V7">
-        <f t="shared" si="14"/>
-        <v>8</v>
-      </c>
-      <c r="W7">
-        <f t="shared" si="15"/>
-        <v>8</v>
-      </c>
       <c r="Y7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="19"/>
+        <v>8</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="20"/>
         <v>315</v>
       </c>
-      <c r="Z7">
-        <v>5</v>
-      </c>
-      <c r="AA7" t="str">
-        <f t="shared" si="17"/>
+      <c r="AD7">
+        <v>5</v>
+      </c>
+      <c r="AE7" t="str">
+        <f t="shared" si="21"/>
         <v>100111011</v>
       </c>
-      <c r="AB7">
-        <f t="shared" si="18"/>
-        <v>9</v>
-      </c>
-      <c r="AC7">
-        <f t="shared" si="19"/>
+      <c r="AF7">
+        <f t="shared" si="22"/>
+        <v>9</v>
+      </c>
+      <c r="AG7">
+        <f t="shared" si="23"/>
+        <v>9</v>
+      </c>
+      <c r="AH7">
+        <f t="shared" si="24"/>
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -963,84 +1081,104 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="G8">
+      <c r="F8">
         <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="5"/>
         <v>42</v>
       </c>
-      <c r="H8">
-        <v>6</v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="5"/>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="6"/>
         <v>101010</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="6"/>
-        <v>6</v>
       </c>
       <c r="K8">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
+      <c r="L8">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
       <c r="M8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="10"/>
         <v>90</v>
       </c>
-      <c r="N8">
-        <v>6</v>
-      </c>
-      <c r="O8" t="str">
-        <f t="shared" si="9"/>
+      <c r="P8">
+        <v>6</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="11"/>
         <v>1011010</v>
       </c>
-      <c r="P8">
-        <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="11"/>
+      <c r="R8">
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="S8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="14"/>
+        <v>7</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="15"/>
         <v>186</v>
       </c>
-      <c r="T8">
-        <v>6</v>
-      </c>
-      <c r="U8" t="str">
-        <f t="shared" si="13"/>
+      <c r="W8">
+        <v>6</v>
+      </c>
+      <c r="X8" t="str">
+        <f t="shared" si="16"/>
         <v>10111010</v>
       </c>
-      <c r="V8">
-        <f t="shared" si="14"/>
-        <v>8</v>
-      </c>
-      <c r="W8">
-        <f t="shared" si="15"/>
-        <v>8</v>
-      </c>
       <c r="Y8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="19"/>
+        <v>8</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="20"/>
         <v>378</v>
       </c>
-      <c r="Z8">
-        <v>6</v>
-      </c>
-      <c r="AA8" t="str">
-        <f t="shared" si="17"/>
+      <c r="AD8">
+        <v>6</v>
+      </c>
+      <c r="AE8" t="str">
+        <f t="shared" si="21"/>
         <v>101111010</v>
       </c>
-      <c r="AB8">
-        <f t="shared" si="18"/>
-        <v>9</v>
-      </c>
-      <c r="AC8">
-        <f t="shared" si="19"/>
+      <c r="AF8">
+        <f t="shared" si="22"/>
+        <v>9</v>
+      </c>
+      <c r="AG8">
+        <f t="shared" si="23"/>
+        <v>9</v>
+      </c>
+      <c r="AH8">
+        <f t="shared" si="24"/>
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1060,84 +1198,104 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="G9">
+      <c r="F9">
         <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="5"/>
         <v>49</v>
       </c>
-      <c r="H9">
-        <v>7</v>
-      </c>
-      <c r="I9" t="str">
-        <f t="shared" si="5"/>
+      <c r="I9">
+        <v>7</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="6"/>
         <v>110001</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="6"/>
-        <v>6</v>
       </c>
       <c r="K9">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
+      <c r="L9">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
       <c r="M9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="10"/>
         <v>105</v>
       </c>
-      <c r="N9">
-        <v>7</v>
-      </c>
-      <c r="O9" t="str">
-        <f t="shared" si="9"/>
+      <c r="P9">
+        <v>7</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="11"/>
         <v>1101001</v>
       </c>
-      <c r="P9">
-        <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="11"/>
+      <c r="R9">
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="S9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="14"/>
+        <v>7</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="15"/>
         <v>217</v>
       </c>
-      <c r="T9">
-        <v>7</v>
-      </c>
-      <c r="U9" t="str">
-        <f t="shared" si="13"/>
+      <c r="W9">
+        <v>7</v>
+      </c>
+      <c r="X9" t="str">
+        <f t="shared" si="16"/>
         <v>11011001</v>
       </c>
-      <c r="V9">
-        <f t="shared" si="14"/>
-        <v>8</v>
-      </c>
-      <c r="W9">
-        <f t="shared" si="15"/>
-        <v>8</v>
-      </c>
       <c r="Y9">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="19"/>
+        <v>8</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="20"/>
         <v>441</v>
       </c>
-      <c r="Z9">
-        <v>7</v>
-      </c>
-      <c r="AA9" t="str">
-        <f t="shared" si="17"/>
+      <c r="AD9">
+        <v>7</v>
+      </c>
+      <c r="AE9" t="str">
+        <f t="shared" si="21"/>
         <v>110111001</v>
       </c>
-      <c r="AB9">
-        <f t="shared" si="18"/>
-        <v>9</v>
-      </c>
-      <c r="AC9">
-        <f t="shared" si="19"/>
+      <c r="AF9">
+        <f t="shared" si="22"/>
+        <v>9</v>
+      </c>
+      <c r="AG9">
+        <f t="shared" si="23"/>
+        <v>9</v>
+      </c>
+      <c r="AH9">
+        <f t="shared" si="24"/>
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1157,84 +1315,104 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="G10">
+      <c r="F10">
         <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="5"/>
         <v>56</v>
       </c>
-      <c r="H10">
-        <v>8</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="5"/>
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="6"/>
         <v>111000</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="6"/>
-        <v>6</v>
       </c>
       <c r="K10">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
+      <c r="L10">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
       <c r="M10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="10"/>
         <v>120</v>
       </c>
-      <c r="N10">
-        <v>8</v>
-      </c>
-      <c r="O10" t="str">
-        <f t="shared" si="9"/>
+      <c r="P10">
+        <v>8</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="11"/>
         <v>1111000</v>
       </c>
-      <c r="P10">
-        <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="11"/>
+      <c r="R10">
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="S10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="15"/>
         <v>248</v>
       </c>
-      <c r="T10">
-        <v>8</v>
-      </c>
-      <c r="U10" t="str">
-        <f t="shared" si="13"/>
+      <c r="W10">
+        <v>8</v>
+      </c>
+      <c r="X10" t="str">
+        <f t="shared" si="16"/>
         <v>11111000</v>
       </c>
-      <c r="V10">
-        <f t="shared" si="14"/>
-        <v>8</v>
-      </c>
-      <c r="W10">
-        <f t="shared" si="15"/>
-        <v>8</v>
-      </c>
       <c r="Y10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="19"/>
+        <v>9</v>
+      </c>
+      <c r="AC10">
+        <f t="shared" si="20"/>
         <v>504</v>
       </c>
-      <c r="Z10">
-        <v>8</v>
-      </c>
-      <c r="AA10" t="str">
-        <f t="shared" si="17"/>
+      <c r="AD10">
+        <v>8</v>
+      </c>
+      <c r="AE10" t="str">
+        <f t="shared" si="21"/>
         <v>111111000</v>
       </c>
-      <c r="AB10">
-        <f t="shared" si="18"/>
-        <v>9</v>
-      </c>
-      <c r="AC10">
-        <f t="shared" si="19"/>
-        <v>9</v>
+      <c r="AF10">
+        <f t="shared" si="22"/>
+        <v>9</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" si="23"/>
+        <v>9</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" si="24"/>
+        <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1254,84 +1432,104 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="G11">
+      <c r="F11">
         <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="5"/>
         <v>63</v>
       </c>
-      <c r="H11">
-        <v>9</v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="5"/>
+      <c r="I11">
+        <v>9</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="6"/>
         <v>111111</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="6"/>
-        <v>6</v>
       </c>
       <c r="K11">
         <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="M11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="10"/>
         <v>135</v>
       </c>
-      <c r="N11">
-        <v>9</v>
-      </c>
-      <c r="O11" t="str">
-        <f t="shared" si="9"/>
+      <c r="P11">
+        <v>9</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="11"/>
         <v>10000111</v>
       </c>
-      <c r="P11">
-        <f t="shared" si="10"/>
-        <v>8</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="11"/>
+      <c r="R11">
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="S11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="15"/>
         <v>279</v>
       </c>
-      <c r="T11">
-        <v>9</v>
-      </c>
-      <c r="U11" t="str">
-        <f t="shared" si="13"/>
+      <c r="W11">
+        <v>9</v>
+      </c>
+      <c r="X11" t="str">
+        <f t="shared" si="16"/>
         <v>100010111</v>
       </c>
-      <c r="V11">
-        <f t="shared" si="14"/>
-        <v>9</v>
-      </c>
-      <c r="W11">
-        <f t="shared" si="15"/>
-        <v>9</v>
-      </c>
       <c r="Y11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="18"/>
+        <v>9</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="19"/>
+        <v>9</v>
+      </c>
+      <c r="AC11">
+        <f t="shared" si="20"/>
         <v>567</v>
       </c>
-      <c r="Z11">
-        <v>9</v>
-      </c>
-      <c r="AA11" t="e">
-        <f t="shared" si="17"/>
+      <c r="AD11">
+        <v>9</v>
+      </c>
+      <c r="AE11" t="e">
+        <f t="shared" si="21"/>
         <v>#NUM!</v>
       </c>
-      <c r="AB11" t="e">
-        <f t="shared" si="18"/>
+      <c r="AF11" t="e">
+        <f t="shared" si="22"/>
         <v>#NUM!</v>
       </c>
-      <c r="AC11">
-        <f t="shared" si="19"/>
+      <c r="AG11">
+        <f t="shared" si="23"/>
         <v>10</v>
       </c>
+      <c r="AH11">
+        <f t="shared" si="24"/>
+        <v>10</v>
+      </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1351,80 +1549,100 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="G12">
+      <c r="F12">
         <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>10</v>
       </c>
-      <c r="I12" t="str">
-        <f t="shared" si="5"/>
+      <c r="J12" t="str">
+        <f t="shared" si="6"/>
         <v>1000110</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="6"/>
-        <v>7</v>
       </c>
       <c r="K12">
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
+      <c r="L12">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
       <c r="M12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="10"/>
         <v>150</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <v>10</v>
       </c>
-      <c r="O12" t="str">
-        <f t="shared" si="9"/>
+      <c r="Q12" t="str">
+        <f t="shared" si="11"/>
         <v>10010110</v>
       </c>
-      <c r="P12">
-        <f t="shared" si="10"/>
-        <v>8</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="11"/>
+      <c r="R12">
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="S12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="15"/>
         <v>310</v>
       </c>
-      <c r="T12">
+      <c r="W12">
         <v>10</v>
       </c>
-      <c r="U12" t="str">
-        <f t="shared" si="13"/>
+      <c r="X12" t="str">
+        <f t="shared" si="16"/>
         <v>100110110</v>
       </c>
-      <c r="V12">
-        <f t="shared" si="14"/>
-        <v>9</v>
-      </c>
-      <c r="W12">
-        <f t="shared" si="15"/>
-        <v>9</v>
-      </c>
       <c r="Y12">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="18"/>
+        <v>9</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="19"/>
+        <v>9</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" si="20"/>
         <v>630</v>
       </c>
-      <c r="Z12">
+      <c r="AD12">
         <v>10</v>
       </c>
-      <c r="AA12" t="e">
-        <f t="shared" si="17"/>
+      <c r="AE12" t="e">
+        <f t="shared" si="21"/>
         <v>#NUM!</v>
       </c>
-      <c r="AB12" t="e">
-        <f t="shared" si="18"/>
+      <c r="AF12" t="e">
+        <f t="shared" si="22"/>
         <v>#NUM!</v>
       </c>
-      <c r="AC12">
-        <f t="shared" si="19"/>
+      <c r="AG12">
+        <f t="shared" si="23"/>
+        <v>10</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="24"/>
         <v>10</v>
       </c>
     </row>

</xml_diff>